<commit_message>
small localization updates and removing useless files
</commit_message>
<xml_diff>
--- a/GameModules/JIAOCHENGMOZU/Localization_JIAOCHENGMOZU.xlsx
+++ b/GameModules/JIAOCHENGMOZU/Localization_JIAOCHENGMOZU.xlsx
@@ -4697,7 +4697,7 @@
       <c r="G99" s="1" t="inlineStr"/>
       <c r="H99" s="1" t="inlineStr">
         <is>
-          <t>Теперь ты может постоять за себя, я перестану направлять тебя.
+          <t>Теперь ты можешь постоять за себя. Я перестану тебя направлять
 Я верю что ты сможешь закончить эту битву с помощью опыта который ты набрал до сего момента.</t>
         </is>
       </c>
@@ -4727,7 +4727,7 @@
       <c r="G100" s="1" t="inlineStr"/>
       <c r="H100" s="1" t="inlineStr">
         <is>
-          <t>Если шанс действия кажется слишком мал, ты можешь использовать удачу чтобы увеличить свои шансы.</t>
+          <t>Если шанс действия кажется слишком малым, ты можешь использовать удачу чтобы усилить его.</t>
         </is>
       </c>
     </row>

</xml_diff>